<commit_message>
Updated CreateEmployee to give better naming
title
</commit_message>
<xml_diff>
--- a/docs/user_stories_ps_team_1.xlsx
+++ b/docs/user_stories_ps_team_1.xlsx
@@ -1,44 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonpearson/Desktop/Summer 2025/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\25su_team1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77B3B2A-409A-B84C-ABD2-E533069BB0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE919FA1-3C31-4FA1-AAB1-9CE568857526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="12" r:id="rId1"/>
     <sheet name="US-1" sheetId="9" r:id="rId2"/>
     <sheet name="US-2" sheetId="11" r:id="rId3"/>
+    <sheet name="US-4" sheetId="13" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="140">
   <si>
     <t>Title</t>
   </si>
@@ -416,6 +406,48 @@
   </si>
   <si>
     <t>View Pay Stubs</t>
+  </si>
+  <si>
+    <t>1. Run app</t>
+  </si>
+  <si>
+    <t>2. Login as a Manager</t>
+  </si>
+  <si>
+    <t>3.  Click Add employee</t>
+  </si>
+  <si>
+    <t>Created a new employee into Employee ArrayList</t>
+  </si>
+  <si>
+    <t>Add an employee (staff).</t>
+  </si>
+  <si>
+    <t>4 . Enter Employee info assign as staff</t>
+  </si>
+  <si>
+    <t>5. Click Add Employee.</t>
+  </si>
+  <si>
+    <t>Add an employee (manager).</t>
+  </si>
+  <si>
+    <t>4 . Enter Employee info assign as Manager</t>
+  </si>
+  <si>
+    <t>Created a new employee into Employee/Manager ArrayList</t>
+  </si>
+  <si>
+    <t>List all managers</t>
+  </si>
+  <si>
+    <t>3.  Click List employees</t>
+  </si>
+  <si>
+    <t>4 . Click List Managers</t>
+  </si>
+  <si>
+    <t>Display list of current managers</t>
   </si>
 </sst>
 </file>
@@ -645,9 +677,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -685,7 +717,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -791,7 +823,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -933,7 +965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -943,33 +975,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DBA430-5312-488B-9461-9DA85FDB31DA}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40" style="2" customWidth="1"/>
-    <col min="7" max="7" width="71.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="10" width="97.5" customWidth="1"/>
+    <col min="7" max="7" width="71.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="97.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1023,7 +1055,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <f>A4+1</f>
         <v>2</v>
@@ -1046,7 +1078,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <f t="shared" ref="A6:A29" si="0">A5+1</f>
         <v>3</v>
@@ -1071,7 +1103,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1096,7 +1128,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1121,7 +1153,7 @@
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1146,7 +1178,7 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1171,7 +1203,7 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1196,7 +1228,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1221,7 +1253,7 @@
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1246,7 +1278,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1269,7 +1301,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1294,7 +1326,7 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1319,7 +1351,7 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1344,7 +1376,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1369,7 +1401,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1394,7 +1426,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1419,7 +1451,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="1:10" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1444,7 +1476,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1469,7 +1501,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
-    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1494,7 +1526,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1517,7 +1549,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1542,7 +1574,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <f>A25+1</f>
         <v>23</v>
@@ -1565,7 +1597,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1590,7 +1622,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1615,7 +1647,7 @@
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1638,7 +1670,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G31" s="2" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" s="2" t="s">
         <v>33</v>
       </c>
@@ -1664,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
@@ -1677,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1690,7 +1722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G35" s="2" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G37" s="2" t="s">
         <v>33</v>
       </c>
@@ -1729,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1742,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G39" s="2" t="s">
         <v>35</v>
       </c>
@@ -1755,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="7:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G40" s="2" t="s">
         <v>36</v>
       </c>
@@ -1781,24 +1813,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="107.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="107.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1806,10 +1838,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1817,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1825,7 +1857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1833,46 +1865,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
@@ -1880,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
@@ -1888,7 +1920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
@@ -1896,19 +1928,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
@@ -1916,19 +1948,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>12</v>
       </c>
@@ -1943,29 +1975,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+      <selection activeCell="E26" sqref="A1:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1973,56 +2008,209 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="C6" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="C11" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F7C54A-CC34-46CC-94FE-A9A160697CD8}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>